<commit_message>
Test case for user registration
</commit_message>
<xml_diff>
--- a/Test Design Specifications/NEW_User_Registration_test_case.xlsx
+++ b/Test Design Specifications/NEW_User_Registration_test_case.xlsx
@@ -548,29 +548,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -856,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
       <selection activeCell="I3" sqref="I3:I13"/>
     </sheetView>
   </sheetViews>
@@ -890,11 +890,11 @@
       <c r="F1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -904,7 +904,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="24"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="9" t="s">
         <v>108</v>
       </c>
@@ -916,13 +916,13 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="19">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -931,150 +931,150 @@
       <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" s="18" t="s">
+      <c r="G3" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
@@ -1101,13 +1101,13 @@
       <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="19">
         <v>2</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="10" t="s">
@@ -1116,72 +1116,72 @@
       <c r="E16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I16" s="18" t="s">
+      <c r="G16" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I16" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="8"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="10" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
@@ -1195,13 +1195,13 @@
       <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="19">
         <v>3</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="10" t="s">
@@ -1210,72 +1210,72 @@
       <c r="E22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I22" s="18" t="s">
+      <c r="G22" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="10" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="23"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
@@ -1289,13 +1289,13 @@
       <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="23">
         <v>4</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="10" t="s">
@@ -1304,72 +1304,72 @@
       <c r="E28" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F28" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G28" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H28" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I28" s="18" t="s">
+      <c r="G28" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I28" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="18"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="8"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
     </row>
     <row r="30" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="18"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="18"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="8"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="18"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F32" s="23"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
     </row>
     <row r="33" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
@@ -1383,13 +1383,13 @@
       <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="19">
         <v>5</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="19" t="s">
         <v>35</v>
       </c>
       <c r="D34" s="10" t="s">
@@ -1398,72 +1398,72 @@
       <c r="E34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="F34" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G34" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I34" s="18" t="s">
+      <c r="G34" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I34" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="10" t="s">
         <v>32</v>
       </c>
       <c r="E36" s="8"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="8"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
     </row>
     <row r="38" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="23"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
     </row>
     <row r="39" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
@@ -1477,13 +1477,13 @@
       <c r="I39" s="8"/>
     </row>
     <row r="40" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="18">
+      <c r="B40" s="19">
         <v>6</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D40" s="10" t="s">
@@ -1492,72 +1492,72 @@
       <c r="E40" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G40" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I40" s="18" t="s">
+      <c r="G40" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I40" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
       <c r="D41" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="8"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E42" s="8"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E43" s="8"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F44" s="23"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
     </row>
     <row r="45" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
@@ -1571,13 +1571,13 @@
       <c r="I45" s="8"/>
     </row>
     <row r="46" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="18">
+      <c r="B46" s="19">
         <v>7</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="19" t="s">
         <v>38</v>
       </c>
       <c r="D46" s="10" t="s">
@@ -1586,72 +1586,72 @@
       <c r="E46" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F46" s="23" t="s">
+      <c r="F46" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G46" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I46" s="18" t="s">
+      <c r="G46" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I46" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
+      <c r="A47" s="21"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
       <c r="D47" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E47" s="8"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E48" s="8"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
       <c r="D49" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E49" s="8"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
     </row>
     <row r="50" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
       <c r="D50" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F50" s="23"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
     </row>
     <row r="51" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
@@ -1665,13 +1665,13 @@
       <c r="I51" s="8"/>
     </row>
     <row r="52" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="18">
+      <c r="B52" s="19">
         <v>8</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="19" t="s">
         <v>41</v>
       </c>
       <c r="D52" s="10" t="s">
@@ -1680,72 +1680,72 @@
       <c r="E52" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F52" s="23" t="s">
+      <c r="F52" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G52" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H52" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I52" s="18" t="s">
+      <c r="G52" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I52" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
       <c r="D53" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E53" s="8"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
       <c r="D54" s="10" t="s">
         <v>42</v>
       </c>
       <c r="E54" s="8"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
+      <c r="A55" s="21"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
       <c r="D55" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E55" s="8"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
     </row>
     <row r="56" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
+      <c r="A56" s="21"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
       <c r="D56" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F56" s="23"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
     </row>
     <row r="57" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
@@ -1759,13 +1759,13 @@
       <c r="I57" s="8"/>
     </row>
     <row r="58" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="18">
+      <c r="B58" s="19">
         <v>9</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="19" t="s">
         <v>44</v>
       </c>
       <c r="D58" s="10" t="s">
@@ -1774,85 +1774,85 @@
       <c r="E58" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F58" s="23" t="s">
+      <c r="F58" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G58" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H58" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I58" s="18" t="s">
+      <c r="G58" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H58" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I58" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
       <c r="D59" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E59" s="8"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
       <c r="D60" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E60" s="8"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
       <c r="D61" s="10" t="s">
         <v>46</v>
       </c>
       <c r="E61" s="8"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
       <c r="D62" s="10" t="s">
         <v>47</v>
       </c>
       <c r="E62" s="8"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
     </row>
     <row r="63" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="17"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
       <c r="D63" s="10" t="s">
         <v>48</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F63" s="23"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
     </row>
     <row r="64" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
@@ -1866,59 +1866,59 @@
       <c r="I64" s="8"/>
     </row>
     <row r="65" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B65" s="18">
+      <c r="B65" s="19">
         <v>10</v>
       </c>
-      <c r="C65" s="18" t="s">
+      <c r="C65" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E65" s="8"/>
-      <c r="F65" s="23" t="s">
+      <c r="F65" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G65" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H65" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I65" s="18" t="s">
+      <c r="G65" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H65" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I65" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="17"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
       <c r="D66" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E66" s="8"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="18"/>
-      <c r="I66" s="18"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
     </row>
     <row r="67" spans="1:9" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
+      <c r="A67" s="21"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
       <c r="D67" s="10" t="s">
         <v>78</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="23"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
     </row>
     <row r="68" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
@@ -1932,13 +1932,13 @@
       <c r="I68" s="8"/>
     </row>
     <row r="69" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B69" s="18">
+      <c r="B69" s="19">
         <v>11</v>
       </c>
-      <c r="C69" s="18" t="s">
+      <c r="C69" s="19" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="10" t="s">
@@ -1947,72 +1947,72 @@
       <c r="E69" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F69" s="23" t="s">
+      <c r="F69" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G69" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H69" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I69" s="18" t="s">
+      <c r="G69" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H69" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I69" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E70" s="8"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="19"/>
+      <c r="I70" s="19"/>
     </row>
     <row r="71" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="17"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
       <c r="D71" s="10" t="s">
         <v>81</v>
       </c>
       <c r="E71" s="8"/>
-      <c r="F71" s="23"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
     </row>
     <row r="72" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
       <c r="D72" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E72" s="8"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
     </row>
     <row r="73" spans="1:9" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="17"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
       <c r="D73" s="10" t="s">
         <v>48</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F73" s="23"/>
-      <c r="G73" s="18"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
     </row>
     <row r="74" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
@@ -2039,13 +2039,13 @@
       <c r="I75" s="8"/>
     </row>
     <row r="76" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
+      <c r="A76" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B76" s="18">
+      <c r="B76" s="19">
         <v>12</v>
       </c>
-      <c r="C76" s="18" t="s">
+      <c r="C76" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D76" s="10" t="s">
@@ -2054,72 +2054,72 @@
       <c r="E76" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F76" s="23" t="s">
+      <c r="F76" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G76" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H76" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I76" s="18" t="s">
+      <c r="G76" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H76" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I76" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="17"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
+      <c r="A77" s="21"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
       <c r="D77" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E77" s="8"/>
-      <c r="F77" s="23"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="17"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
+      <c r="A78" s="21"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
       <c r="D78" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E78" s="8"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="17"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
       <c r="D79" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E79" s="8"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="18"/>
-      <c r="H79" s="18"/>
-      <c r="I79" s="18"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="17"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
+      <c r="A80" s="21"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
       <c r="D80" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F80" s="23"/>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
     </row>
     <row r="81" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
@@ -2133,13 +2133,13 @@
       <c r="I81" s="8"/>
     </row>
     <row r="82" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B82" s="18">
+      <c r="B82" s="19">
         <v>13</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="C82" s="19" t="s">
         <v>53</v>
       </c>
       <c r="D82" s="10" t="s">
@@ -2148,72 +2148,72 @@
       <c r="E82" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F82" s="23" t="s">
+      <c r="F82" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G82" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H82" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I82" s="18" t="s">
+      <c r="G82" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H82" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I82" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="17"/>
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
+      <c r="A83" s="21"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
       <c r="D83" s="10" t="s">
         <v>54</v>
       </c>
       <c r="E83" s="8"/>
-      <c r="F83" s="23"/>
-      <c r="G83" s="18"/>
-      <c r="H83" s="18"/>
-      <c r="I83" s="18"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="19"/>
+      <c r="I83" s="19"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
+      <c r="A84" s="21"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
       <c r="D84" s="10" t="s">
         <v>55</v>
       </c>
       <c r="E84" s="8"/>
-      <c r="F84" s="23"/>
-      <c r="G84" s="18"/>
-      <c r="H84" s="18"/>
-      <c r="I84" s="18"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="19"/>
+      <c r="I84" s="19"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="18"/>
+      <c r="A85" s="21"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
       <c r="D85" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E85" s="8"/>
-      <c r="F85" s="23"/>
-      <c r="G85" s="18"/>
-      <c r="H85" s="18"/>
-      <c r="I85" s="18"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="19"/>
+      <c r="I85" s="19"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="17"/>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
+      <c r="A86" s="21"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
       <c r="D86" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F86" s="23"/>
-      <c r="G86" s="18"/>
-      <c r="H86" s="18"/>
-      <c r="I86" s="18"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="19"/>
+      <c r="I86" s="19"/>
     </row>
     <row r="87" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
@@ -2227,13 +2227,13 @@
       <c r="I87" s="8"/>
     </row>
     <row r="88" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="17" t="s">
+      <c r="A88" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B88" s="18">
+      <c r="B88" s="19">
         <v>14</v>
       </c>
-      <c r="C88" s="18" t="s">
+      <c r="C88" s="19" t="s">
         <v>58</v>
       </c>
       <c r="D88" s="10" t="s">
@@ -2242,72 +2242,72 @@
       <c r="E88" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F88" s="23" t="s">
+      <c r="F88" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G88" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H88" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I88" s="18" t="s">
+      <c r="G88" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H88" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I88" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="17"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
+      <c r="A89" s="21"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
       <c r="D89" s="10" t="s">
         <v>57</v>
       </c>
       <c r="E89" s="8"/>
-      <c r="F89" s="23"/>
-      <c r="G89" s="18"/>
-      <c r="H89" s="18"/>
-      <c r="I89" s="18"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="19"/>
+      <c r="I89" s="19"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
+      <c r="A90" s="21"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
       <c r="D90" s="10" t="s">
         <v>59</v>
       </c>
       <c r="E90" s="8"/>
-      <c r="F90" s="23"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="18"/>
-      <c r="I90" s="18"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="19"/>
+      <c r="I90" s="19"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="17"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="18"/>
+      <c r="A91" s="21"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
       <c r="D91" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E91" s="8"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="18"/>
-      <c r="H91" s="18"/>
-      <c r="I91" s="18"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="19"/>
+      <c r="I91" s="19"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
-      <c r="B92" s="18"/>
-      <c r="C92" s="18"/>
+      <c r="A92" s="21"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
       <c r="D92" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F92" s="23"/>
-      <c r="G92" s="18"/>
-      <c r="H92" s="18"/>
-      <c r="I92" s="18"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="19"/>
+      <c r="H92" s="19"/>
+      <c r="I92" s="19"/>
     </row>
     <row r="93" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
@@ -2321,13 +2321,13 @@
       <c r="I93" s="8"/>
     </row>
     <row r="94" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
+      <c r="A94" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B94" s="18">
+      <c r="B94" s="19">
         <v>15</v>
       </c>
-      <c r="C94" s="18" t="s">
+      <c r="C94" s="19" t="s">
         <v>61</v>
       </c>
       <c r="D94" s="10" t="s">
@@ -2336,72 +2336,72 @@
       <c r="E94" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F94" s="23" t="s">
+      <c r="F94" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G94" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H94" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I94" s="18" t="s">
+      <c r="G94" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H94" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I94" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="17"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
+      <c r="A95" s="21"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="19"/>
       <c r="D95" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E95" s="8"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="18"/>
-      <c r="H95" s="18"/>
-      <c r="I95" s="18"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="19"/>
+      <c r="H95" s="19"/>
+      <c r="I95" s="19"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="17"/>
-      <c r="B96" s="18"/>
-      <c r="C96" s="18"/>
+      <c r="A96" s="21"/>
+      <c r="B96" s="19"/>
+      <c r="C96" s="19"/>
       <c r="D96" s="10" t="s">
         <v>62</v>
       </c>
       <c r="E96" s="8"/>
-      <c r="F96" s="23"/>
-      <c r="G96" s="18"/>
-      <c r="H96" s="18"/>
-      <c r="I96" s="18"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="19"/>
+      <c r="H96" s="19"/>
+      <c r="I96" s="19"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="17"/>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
+      <c r="A97" s="21"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="19"/>
       <c r="D97" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E97" s="8"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="18"/>
-      <c r="H97" s="18"/>
-      <c r="I97" s="18"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="19"/>
+      <c r="H97" s="19"/>
+      <c r="I97" s="19"/>
     </row>
     <row r="98" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
+      <c r="A98" s="21"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="19"/>
       <c r="D98" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F98" s="23"/>
-      <c r="G98" s="18"/>
-      <c r="H98" s="18"/>
-      <c r="I98" s="18"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="19"/>
+      <c r="I98" s="19"/>
     </row>
     <row r="99" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
@@ -2415,13 +2415,13 @@
       <c r="I99" s="8"/>
     </row>
     <row r="100" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="17" t="s">
+      <c r="A100" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B100" s="18">
+      <c r="B100" s="19">
         <v>16</v>
       </c>
-      <c r="C100" s="18" t="s">
+      <c r="C100" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D100" s="10" t="s">
@@ -2430,72 +2430,72 @@
       <c r="E100" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F100" s="23" t="s">
+      <c r="F100" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G100" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H100" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I100" s="18" t="s">
+      <c r="G100" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H100" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I100" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="17"/>
-      <c r="B101" s="18"/>
-      <c r="C101" s="18"/>
+      <c r="A101" s="21"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
       <c r="D101" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E101" s="8"/>
-      <c r="F101" s="23"/>
-      <c r="G101" s="18"/>
-      <c r="H101" s="18"/>
-      <c r="I101" s="18"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="19"/>
+      <c r="H101" s="19"/>
+      <c r="I101" s="19"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
+      <c r="A102" s="21"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="19"/>
       <c r="D102" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E102" s="8"/>
-      <c r="F102" s="23"/>
-      <c r="G102" s="18"/>
-      <c r="H102" s="18"/>
-      <c r="I102" s="18"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="19"/>
+      <c r="I102" s="19"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="17"/>
-      <c r="B103" s="18"/>
-      <c r="C103" s="18"/>
+      <c r="A103" s="21"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="19"/>
       <c r="D103" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E103" s="8"/>
-      <c r="F103" s="23"/>
-      <c r="G103" s="18"/>
-      <c r="H103" s="18"/>
-      <c r="I103" s="18"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="19"/>
+      <c r="H103" s="19"/>
+      <c r="I103" s="19"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="17"/>
-      <c r="B104" s="18"/>
-      <c r="C104" s="18"/>
+      <c r="A104" s="21"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
       <c r="D104" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E104" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F104" s="23"/>
-      <c r="G104" s="18"/>
-      <c r="H104" s="18"/>
-      <c r="I104" s="18"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="19"/>
     </row>
     <row r="105" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8"/>
@@ -2509,13 +2509,13 @@
       <c r="I105" s="8"/>
     </row>
     <row r="106" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
+      <c r="A106" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B106" s="18">
+      <c r="B106" s="19">
         <v>17</v>
       </c>
-      <c r="C106" s="18" t="s">
+      <c r="C106" s="19" t="s">
         <v>67</v>
       </c>
       <c r="D106" s="10" t="s">
@@ -2524,72 +2524,72 @@
       <c r="E106" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F106" s="23" t="s">
+      <c r="F106" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G106" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H106" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I106" s="18" t="s">
+      <c r="G106" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H106" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I106" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="17"/>
-      <c r="B107" s="18"/>
-      <c r="C107" s="18"/>
+      <c r="A107" s="21"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
       <c r="D107" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E107" s="8"/>
-      <c r="F107" s="23"/>
-      <c r="G107" s="18"/>
-      <c r="H107" s="18"/>
-      <c r="I107" s="18"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="19"/>
+      <c r="I107" s="19"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="17"/>
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
+      <c r="A108" s="21"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="19"/>
       <c r="D108" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E108" s="8"/>
-      <c r="F108" s="23"/>
-      <c r="G108" s="18"/>
-      <c r="H108" s="18"/>
-      <c r="I108" s="18"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="19"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="17"/>
-      <c r="B109" s="18"/>
-      <c r="C109" s="18"/>
+      <c r="A109" s="21"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
       <c r="D109" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E109" s="8"/>
-      <c r="F109" s="23"/>
-      <c r="G109" s="18"/>
-      <c r="H109" s="18"/>
-      <c r="I109" s="18"/>
+      <c r="F109" s="20"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="19"/>
+      <c r="I109" s="19"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="17"/>
-      <c r="B110" s="18"/>
-      <c r="C110" s="18"/>
+      <c r="A110" s="21"/>
+      <c r="B110" s="19"/>
+      <c r="C110" s="19"/>
       <c r="D110" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F110" s="23"/>
-      <c r="G110" s="18"/>
-      <c r="H110" s="18"/>
-      <c r="I110" s="18"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="19"/>
+      <c r="H110" s="19"/>
+      <c r="I110" s="19"/>
     </row>
     <row r="111" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="8"/>
@@ -2603,13 +2603,13 @@
       <c r="I111" s="8"/>
     </row>
     <row r="112" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="17" t="s">
+      <c r="A112" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B112" s="22">
         <v>18</v>
       </c>
-      <c r="C112" s="18" t="s">
+      <c r="C112" s="19" t="s">
         <v>70</v>
       </c>
       <c r="D112" s="10" t="s">
@@ -2618,72 +2618,72 @@
       <c r="E112" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F112" s="23" t="s">
+      <c r="F112" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G112" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H112" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I112" s="18" t="s">
+      <c r="G112" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H112" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I112" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="17"/>
+      <c r="A113" s="21"/>
       <c r="B113" s="22"/>
-      <c r="C113" s="18"/>
+      <c r="C113" s="19"/>
       <c r="D113" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E113" s="8"/>
-      <c r="F113" s="23"/>
-      <c r="G113" s="18"/>
-      <c r="H113" s="18"/>
-      <c r="I113" s="18"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="19"/>
+      <c r="I113" s="19"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="17"/>
+      <c r="A114" s="21"/>
       <c r="B114" s="22"/>
-      <c r="C114" s="18"/>
+      <c r="C114" s="19"/>
       <c r="D114" s="10" t="s">
         <v>71</v>
       </c>
       <c r="E114" s="8"/>
-      <c r="F114" s="23"/>
-      <c r="G114" s="18"/>
-      <c r="H114" s="18"/>
-      <c r="I114" s="18"/>
+      <c r="F114" s="20"/>
+      <c r="G114" s="19"/>
+      <c r="H114" s="19"/>
+      <c r="I114" s="19"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="17"/>
+      <c r="A115" s="21"/>
       <c r="B115" s="22"/>
-      <c r="C115" s="18"/>
+      <c r="C115" s="19"/>
       <c r="D115" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E115" s="8"/>
-      <c r="F115" s="23"/>
-      <c r="G115" s="18"/>
-      <c r="H115" s="18"/>
-      <c r="I115" s="18"/>
+      <c r="F115" s="20"/>
+      <c r="G115" s="19"/>
+      <c r="H115" s="19"/>
+      <c r="I115" s="19"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="17"/>
+      <c r="A116" s="21"/>
       <c r="B116" s="22"/>
-      <c r="C116" s="18"/>
+      <c r="C116" s="19"/>
       <c r="D116" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F116" s="23"/>
-      <c r="G116" s="18"/>
-      <c r="H116" s="18"/>
-      <c r="I116" s="18"/>
+      <c r="F116" s="20"/>
+      <c r="G116" s="19"/>
+      <c r="H116" s="19"/>
+      <c r="I116" s="19"/>
     </row>
     <row r="117" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="8"/>
@@ -2710,46 +2710,46 @@
       <c r="I118" s="8"/>
     </row>
     <row r="119" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
+      <c r="A119" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B119" s="18">
+      <c r="B119" s="19">
         <v>19</v>
       </c>
-      <c r="C119" s="18" t="s">
+      <c r="C119" s="19" t="s">
         <v>92</v>
       </c>
       <c r="D119" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E119" s="8"/>
-      <c r="F119" s="23" t="s">
+      <c r="F119" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G119" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H119" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I119" s="18" t="s">
+      <c r="G119" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H119" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I119" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="17"/>
-      <c r="B120" s="18"/>
-      <c r="C120" s="18"/>
+      <c r="A120" s="21"/>
+      <c r="B120" s="19"/>
+      <c r="C120" s="19"/>
       <c r="D120" s="10" t="s">
         <v>85</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F120" s="23"/>
-      <c r="G120" s="18"/>
-      <c r="H120" s="18"/>
-      <c r="I120" s="18"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="19"/>
+      <c r="H120" s="19"/>
+      <c r="I120" s="19"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="8"/>
@@ -2763,46 +2763,46 @@
       <c r="I121" s="8"/>
     </row>
     <row r="122" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="17" t="s">
+      <c r="A122" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B122" s="18">
+      <c r="B122" s="19">
         <v>20</v>
       </c>
-      <c r="C122" s="18" t="s">
+      <c r="C122" s="19" t="s">
         <v>88</v>
       </c>
       <c r="D122" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E122" s="8"/>
-      <c r="F122" s="23" t="s">
+      <c r="F122" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G122" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H122" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I122" s="18" t="s">
+      <c r="G122" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H122" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I122" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="17"/>
-      <c r="B123" s="18"/>
-      <c r="C123" s="18"/>
+      <c r="A123" s="21"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="19"/>
       <c r="D123" s="10" t="s">
         <v>86</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F123" s="23"/>
-      <c r="G123" s="18"/>
-      <c r="H123" s="18"/>
-      <c r="I123" s="18"/>
+      <c r="F123" s="20"/>
+      <c r="G123" s="19"/>
+      <c r="H123" s="19"/>
+      <c r="I123" s="19"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="8"/>
@@ -2816,46 +2816,46 @@
       <c r="I124" s="8"/>
     </row>
     <row r="125" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="17" t="s">
+      <c r="A125" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B125" s="18">
+      <c r="B125" s="19">
         <v>21</v>
       </c>
-      <c r="C125" s="18" t="s">
+      <c r="C125" s="19" t="s">
         <v>89</v>
       </c>
       <c r="D125" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E125" s="8"/>
-      <c r="F125" s="23" t="s">
+      <c r="F125" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G125" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H125" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I125" s="18" t="s">
+      <c r="G125" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H125" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I125" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="17"/>
-      <c r="B126" s="18"/>
-      <c r="C126" s="18"/>
+      <c r="A126" s="21"/>
+      <c r="B126" s="19"/>
+      <c r="C126" s="19"/>
       <c r="D126" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E126" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F126" s="23"/>
-      <c r="G126" s="18"/>
-      <c r="H126" s="18"/>
-      <c r="I126" s="18"/>
+      <c r="F126" s="20"/>
+      <c r="G126" s="19"/>
+      <c r="H126" s="19"/>
+      <c r="I126" s="19"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="8"/>
@@ -2869,46 +2869,46 @@
       <c r="I127" s="8"/>
     </row>
     <row r="128" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="17" t="s">
+      <c r="A128" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B128" s="18">
+      <c r="B128" s="19">
         <v>22</v>
       </c>
-      <c r="C128" s="18" t="s">
+      <c r="C128" s="19" t="s">
         <v>94</v>
       </c>
       <c r="D128" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E128" s="8"/>
-      <c r="F128" s="23" t="s">
+      <c r="F128" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G128" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H128" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I128" s="18" t="s">
+      <c r="G128" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H128" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I128" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="17"/>
-      <c r="B129" s="18"/>
-      <c r="C129" s="18"/>
+      <c r="A129" s="21"/>
+      <c r="B129" s="19"/>
+      <c r="C129" s="19"/>
       <c r="D129" s="10" t="s">
         <v>95</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F129" s="23"/>
-      <c r="G129" s="18"/>
-      <c r="H129" s="18"/>
-      <c r="I129" s="18"/>
+      <c r="F129" s="20"/>
+      <c r="G129" s="19"/>
+      <c r="H129" s="19"/>
+      <c r="I129" s="19"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="8"/>
@@ -2922,46 +2922,46 @@
       <c r="I130" s="8"/>
     </row>
     <row r="131" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="17" t="s">
+      <c r="A131" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B131" s="18">
+      <c r="B131" s="19">
         <v>23</v>
       </c>
-      <c r="C131" s="18" t="s">
+      <c r="C131" s="19" t="s">
         <v>97</v>
       </c>
       <c r="D131" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E131" s="8"/>
-      <c r="F131" s="23" t="s">
+      <c r="F131" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G131" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H131" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I131" s="18" t="s">
+      <c r="G131" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H131" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I131" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="17"/>
-      <c r="B132" s="18"/>
-      <c r="C132" s="18"/>
+      <c r="A132" s="21"/>
+      <c r="B132" s="19"/>
+      <c r="C132" s="19"/>
       <c r="D132" s="10" t="s">
         <v>98</v>
       </c>
       <c r="E132" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F132" s="23"/>
-      <c r="G132" s="18"/>
-      <c r="H132" s="18"/>
-      <c r="I132" s="18"/>
+      <c r="F132" s="20"/>
+      <c r="G132" s="19"/>
+      <c r="H132" s="19"/>
+      <c r="I132" s="19"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="8"/>
@@ -2975,46 +2975,46 @@
       <c r="I133" s="8"/>
     </row>
     <row r="134" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="17" t="s">
+      <c r="A134" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B134" s="18">
+      <c r="B134" s="19">
         <v>24</v>
       </c>
-      <c r="C134" s="18" t="s">
+      <c r="C134" s="19" t="s">
         <v>100</v>
       </c>
       <c r="D134" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E134" s="8"/>
-      <c r="F134" s="23" t="s">
+      <c r="F134" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G134" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H134" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I134" s="18" t="s">
+      <c r="G134" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H134" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I134" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A135" s="17"/>
-      <c r="B135" s="18"/>
-      <c r="C135" s="18"/>
+      <c r="A135" s="21"/>
+      <c r="B135" s="19"/>
+      <c r="C135" s="19"/>
       <c r="D135" s="10" t="s">
         <v>101</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="F135" s="23"/>
-      <c r="G135" s="18"/>
-      <c r="H135" s="18"/>
-      <c r="I135" s="18"/>
+      <c r="F135" s="20"/>
+      <c r="G135" s="19"/>
+      <c r="H135" s="19"/>
+      <c r="I135" s="19"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="8"/>
@@ -3028,46 +3028,46 @@
       <c r="I136" s="8"/>
     </row>
     <row r="137" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="17" t="s">
+      <c r="A137" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B137" s="18">
+      <c r="B137" s="19">
         <v>25</v>
       </c>
-      <c r="C137" s="18" t="s">
+      <c r="C137" s="19" t="s">
         <v>103</v>
       </c>
       <c r="D137" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E137" s="8"/>
-      <c r="F137" s="23" t="s">
+      <c r="F137" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G137" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H137" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I137" s="18" t="s">
+      <c r="G137" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H137" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I137" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="17"/>
-      <c r="B138" s="18"/>
-      <c r="C138" s="18"/>
+      <c r="A138" s="21"/>
+      <c r="B138" s="19"/>
+      <c r="C138" s="19"/>
       <c r="D138" s="10" t="s">
         <v>104</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="F138" s="23"/>
-      <c r="G138" s="18"/>
-      <c r="H138" s="18"/>
-      <c r="I138" s="18"/>
+      <c r="F138" s="20"/>
+      <c r="G138" s="19"/>
+      <c r="H138" s="19"/>
+      <c r="I138" s="19"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="8"/>
@@ -3291,6 +3291,158 @@
     </row>
   </sheetData>
   <mergeCells count="176">
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="B137:B138"/>
+    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G3:G13"/>
+    <mergeCell ref="H3:H13"/>
+    <mergeCell ref="I3:I13"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="A119:A120"/>
+    <mergeCell ref="B119:B120"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B13"/>
+    <mergeCell ref="C3:C13"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="C69:C73"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="A112:A116"/>
+    <mergeCell ref="B112:B116"/>
+    <mergeCell ref="C112:C116"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="B94:B98"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="B100:B104"/>
+    <mergeCell ref="C100:C104"/>
+    <mergeCell ref="A106:A110"/>
+    <mergeCell ref="B106:B110"/>
+    <mergeCell ref="C106:C110"/>
+    <mergeCell ref="A88:A92"/>
+    <mergeCell ref="B88:B92"/>
+    <mergeCell ref="C88:C92"/>
+    <mergeCell ref="F16:F20"/>
+    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="F28:F32"/>
+    <mergeCell ref="G28:G32"/>
+    <mergeCell ref="F40:F44"/>
+    <mergeCell ref="G40:G44"/>
+    <mergeCell ref="F52:F56"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="G76:G80"/>
+    <mergeCell ref="F76:F80"/>
+    <mergeCell ref="F88:F92"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="C58:C63"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="C76:C80"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="H28:H32"/>
+    <mergeCell ref="I28:I32"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="G34:G38"/>
+    <mergeCell ref="H34:H38"/>
+    <mergeCell ref="I34:I38"/>
+    <mergeCell ref="H16:H20"/>
+    <mergeCell ref="I16:I20"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="G22:G26"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="H52:H56"/>
+    <mergeCell ref="I52:I56"/>
+    <mergeCell ref="F58:F63"/>
+    <mergeCell ref="G58:G63"/>
+    <mergeCell ref="H58:H63"/>
+    <mergeCell ref="I58:I63"/>
+    <mergeCell ref="H40:H44"/>
+    <mergeCell ref="I40:I44"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="G46:G50"/>
+    <mergeCell ref="H46:H50"/>
+    <mergeCell ref="I46:I50"/>
+    <mergeCell ref="H76:H80"/>
+    <mergeCell ref="I76:I80"/>
+    <mergeCell ref="F82:F86"/>
+    <mergeCell ref="G82:G86"/>
+    <mergeCell ref="H82:H86"/>
+    <mergeCell ref="I82:I86"/>
+    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="I65:I67"/>
+    <mergeCell ref="F69:F73"/>
+    <mergeCell ref="G69:G73"/>
+    <mergeCell ref="H69:H73"/>
+    <mergeCell ref="I69:I73"/>
+    <mergeCell ref="F100:F104"/>
+    <mergeCell ref="G100:G104"/>
+    <mergeCell ref="H100:H104"/>
+    <mergeCell ref="I100:I104"/>
+    <mergeCell ref="F106:F110"/>
+    <mergeCell ref="G106:G110"/>
+    <mergeCell ref="H106:H110"/>
+    <mergeCell ref="I106:I110"/>
+    <mergeCell ref="G88:G92"/>
+    <mergeCell ref="H88:H92"/>
+    <mergeCell ref="I88:I92"/>
+    <mergeCell ref="F94:F98"/>
+    <mergeCell ref="G94:G98"/>
+    <mergeCell ref="H94:H98"/>
+    <mergeCell ref="I94:I98"/>
+    <mergeCell ref="I125:I126"/>
+    <mergeCell ref="F112:F116"/>
+    <mergeCell ref="G112:G116"/>
+    <mergeCell ref="H112:H116"/>
+    <mergeCell ref="I112:I116"/>
+    <mergeCell ref="F119:F120"/>
+    <mergeCell ref="G119:G120"/>
+    <mergeCell ref="H119:H120"/>
+    <mergeCell ref="I119:I120"/>
     <mergeCell ref="F3:F13"/>
     <mergeCell ref="H131:H132"/>
     <mergeCell ref="I131:I132"/>
@@ -3315,158 +3467,6 @@
     <mergeCell ref="F125:F126"/>
     <mergeCell ref="G125:G126"/>
     <mergeCell ref="H125:H126"/>
-    <mergeCell ref="I125:I126"/>
-    <mergeCell ref="F112:F116"/>
-    <mergeCell ref="G112:G116"/>
-    <mergeCell ref="H112:H116"/>
-    <mergeCell ref="I112:I116"/>
-    <mergeCell ref="F119:F120"/>
-    <mergeCell ref="G119:G120"/>
-    <mergeCell ref="H119:H120"/>
-    <mergeCell ref="I119:I120"/>
-    <mergeCell ref="F100:F104"/>
-    <mergeCell ref="G100:G104"/>
-    <mergeCell ref="H100:H104"/>
-    <mergeCell ref="I100:I104"/>
-    <mergeCell ref="F106:F110"/>
-    <mergeCell ref="G106:G110"/>
-    <mergeCell ref="H106:H110"/>
-    <mergeCell ref="I106:I110"/>
-    <mergeCell ref="G88:G92"/>
-    <mergeCell ref="H88:H92"/>
-    <mergeCell ref="I88:I92"/>
-    <mergeCell ref="F94:F98"/>
-    <mergeCell ref="G94:G98"/>
-    <mergeCell ref="H94:H98"/>
-    <mergeCell ref="I94:I98"/>
-    <mergeCell ref="H76:H80"/>
-    <mergeCell ref="I76:I80"/>
-    <mergeCell ref="F82:F86"/>
-    <mergeCell ref="G82:G86"/>
-    <mergeCell ref="H82:H86"/>
-    <mergeCell ref="I82:I86"/>
-    <mergeCell ref="H65:H67"/>
-    <mergeCell ref="I65:I67"/>
-    <mergeCell ref="F69:F73"/>
-    <mergeCell ref="G69:G73"/>
-    <mergeCell ref="H69:H73"/>
-    <mergeCell ref="I69:I73"/>
-    <mergeCell ref="H52:H56"/>
-    <mergeCell ref="I52:I56"/>
-    <mergeCell ref="F58:F63"/>
-    <mergeCell ref="G58:G63"/>
-    <mergeCell ref="H58:H63"/>
-    <mergeCell ref="I58:I63"/>
-    <mergeCell ref="H40:H44"/>
-    <mergeCell ref="I40:I44"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="G46:G50"/>
-    <mergeCell ref="H46:H50"/>
-    <mergeCell ref="I46:I50"/>
-    <mergeCell ref="H28:H32"/>
-    <mergeCell ref="I28:I32"/>
-    <mergeCell ref="F34:F38"/>
-    <mergeCell ref="G34:G38"/>
-    <mergeCell ref="H34:H38"/>
-    <mergeCell ref="I34:I38"/>
-    <mergeCell ref="H16:H20"/>
-    <mergeCell ref="I16:I20"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="G22:G26"/>
-    <mergeCell ref="H22:H26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="A88:A92"/>
-    <mergeCell ref="B88:B92"/>
-    <mergeCell ref="C88:C92"/>
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="G16:G20"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="G28:G32"/>
-    <mergeCell ref="F40:F44"/>
-    <mergeCell ref="G40:G44"/>
-    <mergeCell ref="F52:F56"/>
-    <mergeCell ref="G52:G56"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="G76:G80"/>
-    <mergeCell ref="F76:F80"/>
-    <mergeCell ref="F88:F92"/>
-    <mergeCell ref="A112:A116"/>
-    <mergeCell ref="B112:B116"/>
-    <mergeCell ref="C112:C116"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="B94:B98"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="B100:B104"/>
-    <mergeCell ref="C100:C104"/>
-    <mergeCell ref="A106:A110"/>
-    <mergeCell ref="B106:B110"/>
-    <mergeCell ref="C106:C110"/>
-    <mergeCell ref="A58:A63"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="C58:C63"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="C69:C73"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="C40:C44"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B13"/>
-    <mergeCell ref="C3:C13"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="C34:C38"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="A119:A120"/>
-    <mergeCell ref="B119:B120"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="B137:B138"/>
-    <mergeCell ref="C137:C138"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G3:G13"/>
-    <mergeCell ref="H3:H13"/>
-    <mergeCell ref="I3:I13"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="B125:B126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>